<commit_message>
CHANGES ON THE CODE , MADE THE STRUCTURE MORE CLEAR TO READ
</commit_message>
<xml_diff>
--- a/4_Outputs/trees_per_citizen.xlsx
+++ b/4_Outputs/trees_per_citizen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>greek_name</t>
   </si>
@@ -196,9 +196,6 @@
     <t>ΜΟΥΣΜΟΥΛΙΑ</t>
   </si>
   <si>
-    <t>ΜΠΕΝΤΖΑΜΙΝ</t>
-  </si>
-  <si>
     <t>ΜΠΡΟΥΣΟΝΕΤΙΑ</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t>ΦΟΙΝΙΚΑΣ</t>
   </si>
   <si>
-    <t>ΦΡΑΓΚΟΣΥΚΙΑ</t>
-  </si>
-  <si>
     <t>ΦΡΑΞΟΣ</t>
   </si>
   <si>
@@ -475,9 +469,6 @@
     <t>Eriobotrya japonica</t>
   </si>
   <si>
-    <t>Ficus benjamina</t>
-  </si>
-  <si>
     <t>Brousonettia papyrifera</t>
   </si>
   <si>
@@ -560,9 +551,6 @@
   </si>
   <si>
     <t>Phoenix canariensis</t>
-  </si>
-  <si>
-    <t>Opuntia ficus-indica</t>
   </si>
   <si>
     <t>Fraxinus angustifolia</t>
@@ -938,7 +926,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -963,7 +951,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>3738</v>
@@ -977,7 +965,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3">
         <v>86</v>
@@ -991,7 +979,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4">
         <v>164</v>
@@ -1005,7 +993,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5">
         <v>741</v>
@@ -1019,7 +1007,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <v>52</v>
@@ -1033,7 +1021,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1047,7 +1035,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1061,7 +1049,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C9">
         <v>29</v>
@@ -1075,7 +1063,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -1089,7 +1077,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1103,7 +1091,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12">
         <v>13</v>
@@ -1117,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C13">
         <v>15</v>
@@ -1131,7 +1119,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14">
         <v>12</v>
@@ -1145,7 +1133,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C15">
         <v>22</v>
@@ -1159,7 +1147,7 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C16">
         <v>116</v>
@@ -1173,7 +1161,7 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C17">
         <v>46</v>
@@ -1187,7 +1175,7 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C18">
         <v>185</v>
@@ -1201,7 +1189,7 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C19">
         <v>16</v>
@@ -1215,7 +1203,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C20">
         <v>88</v>
@@ -1229,7 +1217,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C21">
         <v>12</v>
@@ -1243,7 +1231,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C22">
         <v>633</v>
@@ -1257,7 +1245,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23">
         <v>27</v>
@@ -1271,7 +1259,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C24">
         <v>727</v>
@@ -1285,7 +1273,7 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C25">
         <v>515</v>
@@ -1299,7 +1287,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1313,7 +1301,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C27">
         <v>204</v>
@@ -1327,7 +1315,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C28">
         <v>280</v>
@@ -1341,7 +1329,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C29">
         <v>31</v>
@@ -1355,7 +1343,7 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1369,7 +1357,7 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -1383,7 +1371,7 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C32">
         <v>887</v>
@@ -1397,7 +1385,7 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C33">
         <v>31</v>
@@ -1411,7 +1399,7 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1425,7 +1413,7 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C35">
         <v>180</v>
@@ -1439,7 +1427,7 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C36">
         <v>10</v>
@@ -1453,7 +1441,7 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C37">
         <v>9</v>
@@ -1467,7 +1455,7 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C38">
         <v>1115</v>
@@ -1481,7 +1469,7 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C39">
         <v>31</v>
@@ -1495,7 +1483,7 @@
         <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C40">
         <v>702</v>
@@ -1509,7 +1497,7 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C41">
         <v>2341</v>
@@ -1523,7 +1511,7 @@
         <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C42">
         <v>58</v>
@@ -1537,7 +1525,7 @@
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C43">
         <v>29</v>
@@ -1551,7 +1539,7 @@
         <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C44">
         <v>8</v>
@@ -1565,7 +1553,7 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C45">
         <v>337</v>
@@ -1579,7 +1567,7 @@
         <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C46">
         <v>3</v>
@@ -1593,7 +1581,7 @@
         <v>49</v>
       </c>
       <c r="B47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C47">
         <v>5</v>
@@ -1607,7 +1595,7 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C48">
         <v>18</v>
@@ -1621,7 +1609,7 @@
         <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C49">
         <v>827</v>
@@ -1635,7 +1623,7 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C50">
         <v>1083</v>
@@ -1649,7 +1637,7 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C51">
         <v>2881</v>
@@ -1663,7 +1651,7 @@
         <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C52">
         <v>23</v>
@@ -1677,7 +1665,7 @@
         <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -1691,7 +1679,7 @@
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C54">
         <v>94</v>
@@ -1705,7 +1693,7 @@
         <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C55">
         <v>47</v>
@@ -1719,7 +1707,7 @@
         <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C56">
         <v>303</v>
@@ -1733,7 +1721,7 @@
         <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C57">
         <v>56</v>
@@ -1747,13 +1735,13 @@
         <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>0.0003792568446457397</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1761,13 +1749,13 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C59">
-        <v>121</v>
+        <v>1536</v>
       </c>
       <c r="D59">
-        <v>0.0003792568446457397</v>
+        <v>0.004814367879139306</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1775,13 +1763,13 @@
         <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C60">
-        <v>1536</v>
+        <v>12</v>
       </c>
       <c r="D60">
-        <v>0.004814367879139306</v>
+        <v>3.761224905577583E-05</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1789,13 +1777,13 @@
         <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C61">
-        <v>12</v>
+        <v>151</v>
       </c>
       <c r="D61">
-        <v>3.761224905577583E-05</v>
+        <v>0.0004732874672851792</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1803,13 +1791,13 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C62">
-        <v>151</v>
+        <v>3</v>
       </c>
       <c r="D62">
-        <v>0.0004732874672851792</v>
+        <v>9.403062263943958E-06</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1817,13 +1805,13 @@
         <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C63">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D63">
-        <v>9.403062263943958E-06</v>
+        <v>0.000294629284270244</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1831,13 +1819,13 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C64">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D64">
-        <v>0.000294629284270244</v>
+        <v>0.0002664200974784121</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1845,13 +1833,13 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C65">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="D65">
-        <v>0.0002664200974784121</v>
+        <v>6.268708175962639E-05</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1859,13 +1847,13 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C66">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="D66">
-        <v>6.268708175962639E-05</v>
+        <v>0.0001974643075428231</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1873,13 +1861,13 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C67">
-        <v>63</v>
+        <v>259</v>
       </c>
       <c r="D67">
-        <v>0.0001974643075428231</v>
+        <v>0.0008117977087871617</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1887,13 +1875,13 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C68">
-        <v>259</v>
+        <v>1813</v>
       </c>
       <c r="D68">
-        <v>0.0008117977087871617</v>
+        <v>0.005682583961510132</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1901,13 +1889,13 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C69">
-        <v>1813</v>
+        <v>12</v>
       </c>
       <c r="D69">
-        <v>0.005682583961510132</v>
+        <v>3.761224905577583E-05</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1915,13 +1903,13 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C70">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D70">
-        <v>3.761224905577583E-05</v>
+        <v>1.56717704399066E-05</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1929,13 +1917,13 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C71">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D71">
-        <v>1.56717704399066E-05</v>
+        <v>0.0001128367471673275</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1943,13 +1931,13 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C72">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>0.0001128367471673275</v>
+        <v>3.134354087981319E-06</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1957,13 +1945,13 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>154</v>
       </c>
       <c r="D73">
-        <v>3.134354087981319E-06</v>
+        <v>0.0004826905295491232</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1971,13 +1959,13 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C74">
-        <v>154</v>
+        <v>5785</v>
       </c>
       <c r="D74">
-        <v>0.0004826905295491232</v>
+        <v>0.01813223839897193</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1985,13 +1973,13 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C75">
-        <v>5785</v>
+        <v>98</v>
       </c>
       <c r="D75">
-        <v>0.01813223839897193</v>
+        <v>0.0003071667006221693</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1999,13 +1987,13 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C76">
-        <v>98</v>
+        <v>3641</v>
       </c>
       <c r="D76">
-        <v>0.0003071667006221693</v>
+        <v>0.01141218323433998</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2013,13 +2001,13 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C77">
-        <v>3641</v>
+        <v>781</v>
       </c>
       <c r="D77">
-        <v>0.01141218323433998</v>
+        <v>0.00244793054271341</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2027,13 +2015,13 @@
         <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C78">
-        <v>781</v>
+        <v>7</v>
       </c>
       <c r="D78">
-        <v>0.00244793054271341</v>
+        <v>2.194047861586923E-05</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2041,13 +2029,13 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C79">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D79">
-        <v>2.194047861586923E-05</v>
+        <v>3.134354087981319E-06</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2055,13 +2043,13 @@
         <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D80">
-        <v>3.134354087981319E-06</v>
+        <v>1.253741635192528E-05</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2069,13 +2057,13 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C81">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D81">
-        <v>1.253741635192528E-05</v>
+        <v>2.820918679183187E-05</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2083,13 +2071,13 @@
         <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C82">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="D82">
-        <v>2.820918679183187E-05</v>
+        <v>0.0001598520584870473</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2097,13 +2085,13 @@
         <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C83">
-        <v>51</v>
+        <v>1071</v>
       </c>
       <c r="D83">
-        <v>0.0001598520584870473</v>
+        <v>0.003356893228227993</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2111,13 +2099,13 @@
         <v>86</v>
       </c>
       <c r="B84" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C84">
-        <v>1071</v>
+        <v>1010</v>
       </c>
       <c r="D84">
-        <v>0.003356893228227993</v>
+        <v>0.003165697628861132</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2125,13 +2113,13 @@
         <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C85">
-        <v>1010</v>
+        <v>44</v>
       </c>
       <c r="D85">
-        <v>0.003165697628861132</v>
+        <v>0.000137911579871178</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2139,13 +2127,13 @@
         <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C86">
-        <v>44</v>
+        <v>687</v>
       </c>
       <c r="D86">
-        <v>0.000137911579871178</v>
+        <v>0.002153301258443166</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2153,13 +2141,13 @@
         <v>89</v>
       </c>
       <c r="B87" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>6.268708175962639E-06</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2167,13 +2155,13 @@
         <v>90</v>
       </c>
       <c r="B88" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C88">
-        <v>687</v>
+        <v>250</v>
       </c>
       <c r="D88">
-        <v>0.002153301258443166</v>
+        <v>0.0007835885219953298</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2181,13 +2169,13 @@
         <v>91</v>
       </c>
       <c r="B89" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C89">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="D89">
-        <v>6.268708175962639E-06</v>
+        <v>0.0001441802880471407</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2195,13 +2183,13 @@
         <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C90">
-        <v>250</v>
+        <v>4794</v>
       </c>
       <c r="D90">
-        <v>0.0007835885219953298</v>
+        <v>0.01502609349778244</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2209,51 +2197,23 @@
         <v>93</v>
       </c>
       <c r="B91" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C91">
-        <v>46</v>
+        <v>352</v>
       </c>
       <c r="D91">
-        <v>0.0001441802880471407</v>
+        <v>0.001103292638969424</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>94</v>
       </c>
-      <c r="B92" t="s">
-        <v>187</v>
-      </c>
       <c r="C92">
-        <v>4794</v>
+        <v>41859</v>
       </c>
       <c r="D92">
-        <v>0.01502609349778244</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" t="s">
-        <v>95</v>
-      </c>
-      <c r="B93" t="s">
-        <v>188</v>
-      </c>
-      <c r="C93">
-        <v>352</v>
-      </c>
-      <c r="D93">
-        <v>0.001103292638969424</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94" t="s">
-        <v>96</v>
-      </c>
-      <c r="C94">
-        <v>41859</v>
-      </c>
-      <c r="D94">
         <v>0.13120092776881</v>
       </c>
     </row>

</xml_diff>